<commit_message>
commit after login and batch
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0019cff6cfb10f79/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepthi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{DA5A7A5A-3E78-481A-A6D0-6CA7CAE9ABE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A520DF2D-6286-4CD5-82D7-D60C409402B0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1761E6-154D-43F0-9EE0-54FBEF4939CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F06861D2-CA69-471A-8E66-3777D41CE6CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{F06861D2-CA69-471A-8E66-3777D41CE6CB}"/>
   </bookViews>
   <sheets>
     <sheet name="program" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="user" sheetId="4" r:id="rId3"/>
     <sheet name="student" sheetId="6" r:id="rId4"/>
     <sheet name="staff" sheetId="7" r:id="rId5"/>
+    <sheet name="login" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,8 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>email</t>
   </si>
@@ -64,13 +63,37 @@
   </si>
   <si>
     <t>ninjahackers01@gmail.com</t>
+  </si>
+  <si>
+    <t>mytesting</t>
+  </si>
+  <si>
+    <t>bhuvee@mail.com</t>
+  </si>
+  <si>
+    <t>UIHackathon@02</t>
+  </si>
+  <si>
+    <t>sdetorganizers@gmail.com</t>
+  </si>
+  <si>
+    <t>invalidPassword</t>
+  </si>
+  <si>
+    <t>invalidUsername</t>
+  </si>
+  <si>
+    <t>validPassword</t>
+  </si>
+  <si>
+    <t>validUserName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +105,13 @@
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -102,14 +132,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -123,10 +156,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -484,7 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB07C4CA-1828-4E68-9B46-E4C24480E8B6}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -586,4 +615,52 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30E1EFD-3D77-470A-A0E4-9BC873C51FC1}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{D562EEF7-8D6A-4D33-8FA4-D1AF53ED4CB7}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C64F8DC0-B9AC-4752-9EBB-99CFB2D70618}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{454F7D7B-1603-4D51-8F0C-87DA65D719DE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>